<commit_message>
migrate to new kb
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/sim_test_wc_kb.xlsx
+++ b/tests/multialgorithm/fixtures/sim_test_wc_kb.xlsx
@@ -5,13 +5,13 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_sim/tmp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arthur_at_sinai/gitOnMyLaptopLocal/wc_dev_repos/wc_sim/tests/multialgorithm/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13400" yWindow="460" windowWidth="13240" windowHeight="5540" tabRatio="500" firstSheet="3" activeTab="3"/>
-    <workbookView xWindow="12400" yWindow="6020" windowWidth="15020" windowHeight="5680" tabRatio="500" firstSheet="10" activeTab="11"/>
-    <workbookView xWindow="13840" yWindow="11980" windowWidth="13460" windowHeight="5860" tabRatio="500" firstSheet="10" activeTab="12"/>
+    <workbookView xWindow="14740" yWindow="460" windowWidth="13220" windowHeight="12640" tabRatio="500" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="15400" yWindow="6060" windowWidth="12380" windowHeight="5700" tabRatio="500" firstSheet="7" activeTab="10"/>
+    <workbookView xWindow="14920" yWindow="12160" windowWidth="12380" windowHeight="5680" tabRatio="500" firstSheet="10" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="Knowledge base" sheetId="1" r:id="rId1"/>
@@ -25,25 +25,27 @@
     <sheet name="Gene loci" sheetId="9" r:id="rId9"/>
     <sheet name="Protein species types" sheetId="10" r:id="rId10"/>
     <sheet name="Complex species types" sheetId="11" r:id="rId11"/>
-    <sheet name="Reactions" sheetId="12" r:id="rId12"/>
-    <sheet name="Rate laws" sheetId="17" r:id="rId13"/>
-    <sheet name="Properties" sheetId="13" r:id="rId14"/>
-    <sheet name="Observables" sheetId="14" r:id="rId15"/>
+    <sheet name="Concentrations" sheetId="18" r:id="rId12"/>
+    <sheet name="Reactions" sheetId="12" r:id="rId13"/>
+    <sheet name="Rate laws" sheetId="17" r:id="rId14"/>
+    <sheet name="Properties" sheetId="13" r:id="rId15"/>
+    <sheet name="Observables" sheetId="14" r:id="rId16"/>
+    <sheet name="References" sheetId="19" r:id="rId17"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Cell!$A$1:$A$3</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Cell!$A$1:$A$4</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Compartments!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Complex species types'!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'DNA species types'!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Complex species types'!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'DNA species types'!$A$1:$G$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'Gene loci'!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Knowledge base'!$A$1:$B$9</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Metabolite species types'!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Observables!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Metabolite species types'!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">Observables!$A$1:$F$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'Promoter loci'!$A$1:$I$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">Properties!$A$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Protein species types'!$A$1:$I$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">Reactions!$A$1:$E$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Rna species types'!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">Properties!$A$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Protein species types'!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Reactions!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'Rna species types'!$A$1:$H$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Transcription unit loci'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
@@ -59,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="121">
   <si>
     <t>Id</t>
   </si>
@@ -91,13 +93,7 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Volume</t>
-  </si>
-  <si>
     <t>Structure</t>
-  </si>
-  <si>
-    <t>Concentration</t>
   </si>
   <si>
     <t>Half life</t>
@@ -408,13 +404,34 @@
   </si>
   <si>
     <t>"7"</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>standard id</t>
+  </si>
+  <si>
+    <t>ref_1</t>
+  </si>
+  <si>
+    <t>10.1000/xyz123</t>
+  </si>
+  <si>
+    <t>Taxon</t>
+  </si>
+  <si>
+    <t>Volumetric fraction</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -449,8 +466,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -462,8 +502,20 @@
         <fgColor rgb="FFCCCCCC"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFCCCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -471,12 +523,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -498,10 +564,38 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="7">
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -806,10 +900,10 @@
     <sheetView workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.59765625" customWidth="1"/>
-    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -817,7 +911,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -825,7 +919,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -887,10 +981,12 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -900,29 +996,29 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="I1" s="18" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1"/>
+  <autoFilter ref="A1:H1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -932,10 +1028,12 @@
   <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -945,57 +1043,96 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="J1" s="18" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1"/>
+  <autoFilter ref="A1:I1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:AMD1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="2"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="8.83203125" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1018" s="13" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>114</v>
+      </c>
+      <c r="AMC1" s="14"/>
+      <c r="AMD1" s="14"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView topLeftCell="C1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="20.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.19921875" customWidth="1"/>
+    <col min="1" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1003,97 +1140,100 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>61</v>
       </c>
-      <c r="B2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B3" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" t="s">
-        <v>59</v>
-      </c>
-      <c r="E3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>63</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>64</v>
       </c>
-      <c r="C4" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="C5" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C6" t="s">
         <v>65</v>
-      </c>
-      <c r="B5" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E5" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B6" t="s">
-        <v>54</v>
-      </c>
-      <c r="C6" t="s">
-        <v>67</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" t="s">
         <v>112</v>
-      </c>
-      <c r="B7" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" t="s">
-        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1102,9 +1242,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
@@ -1112,85 +1252,88 @@
       <selection pane="bottomLeft"/>
       <selection pane="bottomRight" activeCell="E1" sqref="E1"/>
     </sheetView>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="2">
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="2">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.3984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.59765625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.19921875" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="7" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>73</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>75</v>
       </c>
       <c r="F1" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" s="18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D2" s="7"/>
       <c r="E2" s="7"/>
       <c r="F2" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="7"/>
       <c r="F3" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D4" s="7">
         <v>1</v>
@@ -1199,66 +1342,66 @@
         <v>2</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -1266,26 +1409,28 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="E2" sqref="A1:E5"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="19.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1293,72 +1438,75 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C2" s="5">
         <v>1.0000000000000001E-15</v>
       </c>
       <c r="D2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" t="s">
         <v>93</v>
-      </c>
-      <c r="E2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B3" t="s">
-        <v>95</v>
       </c>
       <c r="C3" s="5">
         <v>10000000</v>
       </c>
       <c r="D3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B4" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B4" t="s">
-        <v>98</v>
       </c>
       <c r="C4">
         <v>0.7</v>
       </c>
       <c r="D4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B5" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B5" t="s">
-        <v>101</v>
       </c>
       <c r="C5">
         <v>1200</v>
       </c>
       <c r="D5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1367,17 +1515,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="G1" sqref="G1"/>
+    </sheetView>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1385,16 +1535,19 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="G1" s="18" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1403,17 +1556,60 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="A3:B4"/>
+    </sheetView>
     <sheetView workbookViewId="1"/>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="16.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="14"/>
+    <col min="2" max="2" width="18.5" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="8.83203125" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+    <sheetView workbookViewId="1">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+    <sheetView workbookViewId="2"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="16.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1421,7 +1617,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1429,70 +1625,79 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:A3"/>
+  <autoFilter ref="A1:A4"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:D2"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.3984375" customWidth="1"/>
-    <col min="4" max="4" width="18.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>10</v>
+      <c r="C1" s="19" t="s">
+        <v>120</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="18" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="4" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="5">
-        <v>1.0000000000000001E-18</v>
-      </c>
+      <c r="C3" s="4"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1"/>
@@ -1505,21 +1710,21 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
-    </sheetView>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
-      <selection activeCell="A6" sqref="A6"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+    </sheetView>
+    <sheetView topLeftCell="C1" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="1">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" style="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1529,94 +1734,79 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="F1" s="18" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>110</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
+        <v>49</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D3">
-        <v>1</v>
+        <v>109</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4" t="s">
-        <v>106</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
+        <v>52</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5" t="s">
-        <v>105</v>
-      </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>62</v>
+        <v>53</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E5" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B6" t="s">
+        <v>105</v>
+      </c>
+      <c r="C6" s="21" t="s">
         <v>107</v>
       </c>
-      <c r="C6" t="s">
-        <v>109</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1"/>
+  <autoFilter ref="A1:E1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -1626,10 +1816,12 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1639,67 +1831,72 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="H1" s="18" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1"/>
+  <autoFilter ref="A1:G1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1710,41 +1907,46 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1758,10 +1960,12 @@
   <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -1771,70 +1975,75 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="I1" s="18" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1"/>
+  <autoFilter ref="A1:H1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:J1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="J1" sqref="J1"/>
+    </sheetView>
     <sheetView workbookViewId="2"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.796875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>9</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>